<commit_message>
feat: add course_code column to Major model and update data loader
- Added course_code column in Major model (models.py) like BP004
- Updated data_loader.py to load course_code from major sequence files
</commit_message>
<xml_diff>
--- a/Reference_Material/Essential_Data/Sequence export (MJD-FINEC).xlsx
+++ b/Reference_Material/Essential_Data/Sequence export (MJD-FINEC).xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8CDF7453620923A0ED0ADEBD13C3EE9E180E5844" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/24409105_student_uwa_edu_au/Documents/UWA/4th semester/cits5206 capstone/AI-Study-Planner-Group8/Reference_Material/Essential_Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8CDF7453620923A0ED0ADEBD13C3EE9E180E5844" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC6CDEA0-3321-43A0-B99D-BA779A0D2CCF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence export" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sequence export'!$A$3:$I$25</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sequence export'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="999999" fullCalcOnLoad="1" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -517,7 +522,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -534,6 +539,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -596,7 +607,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -898,24 +909,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
     <col min="4" max="6" width="80" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="9" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -928,7 +938,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -941,7 +951,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -970,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>186</v>
       </c>
@@ -999,7 +1009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>187</v>
       </c>
@@ -1028,7 +1038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>397</v>
       </c>
@@ -1057,7 +1067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>536</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>215</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>192</v>
       </c>
@@ -1144,7 +1154,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>206</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>207</v>
       </c>
@@ -1202,7 +1212,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>497</v>
       </c>
@@ -1231,7 +1241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>7746</v>
       </c>
@@ -1260,7 +1270,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>209</v>
       </c>
@@ -1289,7 +1299,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>212</v>
       </c>
@@ -1318,7 +1328,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>232</v>
       </c>
@@ -1347,7 +1357,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>525</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>231</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>326</v>
       </c>
@@ -1434,7 +1444,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>328</v>
       </c>
@@ -1463,7 +1473,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>506</v>
       </c>
@@ -1492,7 +1502,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>521</v>
       </c>
@@ -1521,7 +1531,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>526</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>59</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7325</v>
       </c>
@@ -1611,8 +1621,9 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A3:I25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3543307086614173" right="0.3543307086614173" top="0.3543307086614173" bottom="0.3543307086614173" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;BGenerated by CAIDi &amp;D &amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -1620,18 +1631,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1773,13 +1784,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC103695-8C60-47C0-8508-B7180910419E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{417EC130-C367-4B15-A996-3B59E943B9BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{417EC130-C367-4B15-A996-3B59E943B9BE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC103695-8C60-47C0-8508-B7180910419E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80D067CA-D43F-4ADA-886B-36A502CF6520}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80D067CA-D43F-4ADA-886B-36A502CF6520}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f5437da9-3489-479d-94d5-fe8d702a56ae"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>